<commit_message>
minor changes to test sheet
</commit_message>
<xml_diff>
--- a/tests/test_sheets/eng.xlsx
+++ b/tests/test_sheets/eng.xlsx
@@ -12,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Attikus!$A$2:$K$5</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>ISBN</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>The Best Science fiction of 2019</t>
+  </si>
+  <si>
+    <t>13</t>
   </si>
 </sst>
 </file>
@@ -244,7 +247,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -286,6 +289,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="0,0_x000d__x000a_NA_x000d__x000a_" xfId="1"/>
@@ -596,7 +602,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,8 +762,8 @@
       <c r="L4" s="9">
         <v>2019</v>
       </c>
-      <c r="M4" s="7">
-        <v>13</v>
+      <c r="M4" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="N4" s="7">
         <v>11.99</v>

</xml_diff>

<commit_message>
title forced to str (#77)
</commit_message>
<xml_diff>
--- a/tests/test_sheets/eng.xlsx
+++ b/tests/test_sheets/eng.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>ISBN</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>13</t>
+  </si>
+  <si>
+    <t>Orwell, George</t>
   </si>
 </sst>
 </file>
@@ -247,7 +250,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -290,6 +293,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -599,10 +608,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,7 +630,7 @@
     <col min="12" max="12" width="11.140625" style="1" customWidth="1"/>
     <col min="13" max="13" width="13.42578125" style="1" customWidth="1"/>
     <col min="14" max="14" width="13.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" style="16" customWidth="1"/>
     <col min="16" max="16" width="24.85546875" style="1" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -672,7 +681,7 @@
       <c r="N2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="17" t="s">
         <v>10</v>
       </c>
       <c r="P2" s="7" t="s">
@@ -720,7 +729,7 @@
       <c r="N3" s="12">
         <v>25</v>
       </c>
-      <c r="O3" s="7">
+      <c r="O3" s="17">
         <v>5060099503825</v>
       </c>
       <c r="P3" s="14" t="s">
@@ -768,7 +777,7 @@
       <c r="N4" s="7">
         <v>11.99</v>
       </c>
-      <c r="O4" s="7">
+      <c r="O4" s="17">
         <v>5060099503826</v>
       </c>
       <c r="P4" s="14" t="s">
@@ -806,10 +815,39 @@
         <v>15.99</v>
       </c>
       <c r="N5" s="7"/>
-      <c r="O5" s="7">
+      <c r="O5" s="17">
         <v>5060099503827</v>
       </c>
       <c r="P5" s="7"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1984</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="1">
+        <v>2018</v>
+      </c>
+      <c r="M6" s="1">
+        <v>9.99</v>
+      </c>
+      <c r="N6" s="1">
+        <v>7.99</v>
+      </c>
+      <c r="O6" s="17">
+        <v>5060099503828</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:K5"/>

</xml_diff>

<commit_message>
comment col added to sheet mapping (#78)
</commit_message>
<xml_diff>
--- a/tests/test_sheets/eng.xlsx
+++ b/tests/test_sheets/eng.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>ISBN</t>
   </si>
@@ -146,6 +146,24 @@
   </si>
   <si>
     <t>Orwell, George</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>misc</t>
+  </si>
+  <si>
+    <t>order 3</t>
+  </si>
+  <si>
+    <t>order 4</t>
+  </si>
+  <si>
+    <t>juv</t>
+  </si>
+  <si>
+    <t>rush</t>
   </si>
 </sst>
 </file>
@@ -250,7 +268,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -299,6 +317,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -608,10 +632,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,10 +659,10 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -681,14 +705,20 @@
       <c r="N2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="Q2" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="19" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
@@ -735,8 +765,14 @@
       <c r="P3" s="14" t="s">
         <v>37</v>
       </c>
+      <c r="Q3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
@@ -783,8 +819,11 @@
       <c r="P4" s="14" t="s">
         <v>38</v>
       </c>
+      <c r="Q4" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -819,8 +858,11 @@
         <v>5060099503827</v>
       </c>
       <c r="P5" s="7"/>
+      <c r="Q5" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>42</v>
       </c>

</xml_diff>